<commit_message>
modified:   .ipynb_checkpoints/Part1_Sequence-checkpoint.ipynb 	modified:   Part1_Sequence.ipynb 	modified:   hw3/.ipynb_checkpoints/answers-checkpoint.py 	modified:   hw3/.ipynb_checkpoints/training-checkpoint.py 	modified:   hw3/__pycache__/answers.cpython-38.pyc 	modified:   hw3/__pycache__/training.cpython-38.pyc 	modified:   hw3/answers.py 	modified:   hw3/training.py 	modified:   my_part1_checkpoints/experiments docomentaion.xlsx 	renamed:    checkpoints/rnn.pt -> my_part1_checkpoints/rnn_2.pt 	new file:   my_part1_checkpoints/rnn_4.pt 	new file:   my_part1_checkpoints/rnn_6.pt 	new file:   my_part1_checkpoints/rnn_8.pt
</commit_message>
<xml_diff>
--- a/my_part1_checkpoints/experiments docomentaion.xlsx
+++ b/my_part1_checkpoints/experiments docomentaion.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aviv\Documents\deep_learning_git\Deep_Learning_hw3\my_part1_checkpoints\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8EE58FD-CF54-4622-8756-0365995ECDBD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1866BF6B-E8B7-4EC5-A798-00DEC7F56FDA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32715" yWindow="3060" windowWidth="17355" windowHeight="21000" xr2:uid="{4AF1D7C4-9F9F-406B-A4B4-FD5F768A1BA3}"/>
+    <workbookView xWindow="22275" yWindow="960" windowWidth="20250" windowHeight="21000" xr2:uid="{4AF1D7C4-9F9F-406B-A4B4-FD5F768A1BA3}"/>
   </bookViews>
   <sheets>
     <sheet name="גיליון1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="29">
   <si>
     <t>batch_size</t>
   </si>
@@ -82,16 +82,62 @@
   </si>
   <si>
     <t>8/50</t>
+  </si>
+  <si>
+    <t>50/50</t>
+  </si>
+  <si>
+    <t>28/50</t>
+  </si>
+  <si>
+    <t>65/100</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>95% train data</t>
+  </si>
+  <si>
+    <t>~63</t>
+  </si>
+  <si>
+    <t>38/50</t>
+  </si>
+  <si>
+    <t>100 epoch</t>
+  </si>
+  <si>
+    <t>run On</t>
+  </si>
+  <si>
+    <t>server</t>
+  </si>
+  <si>
+    <t>PC</t>
+  </si>
+  <si>
+    <t>73/100</t>
+  </si>
+  <si>
+    <t>10/100</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="177"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="177"/>
@@ -130,39 +176,45 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="15">
+  <dxfs count="17">
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -191,13 +243,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{075A1864-AD5B-4FE4-BDE0-86A04725ED44}" name="טבלה1" displayName="טבלה1" ref="A1:N3" totalsRowShown="0" dataDxfId="1">
-  <autoFilter ref="A1:N3" xr:uid="{86CC994D-4FD3-4DBF-8BD4-8671CE84E166}"/>
-  <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{6D5CF608-DCFD-4A92-A596-E8063172E174}" name="serial No" dataDxfId="14"/>
-    <tableColumn id="2" xr3:uid="{C0209DF9-846E-4857-B58B-B8541011985F}" name="runNo" dataDxfId="13"/>
-    <tableColumn id="3" xr3:uid="{0E30CBAC-72EE-4AD2-A47C-82B32671EA5E}" name="prev" dataDxfId="12"/>
-    <tableColumn id="14" xr3:uid="{0226C407-085D-4DCB-8736-D2AF531847FD}" name="final epoch" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{075A1864-AD5B-4FE4-BDE0-86A04725ED44}" name="טבלה1" displayName="טבלה1" ref="A1:P13" totalsRowShown="0" dataDxfId="16">
+  <autoFilter ref="A1:P13" xr:uid="{86CC994D-4FD3-4DBF-8BD4-8671CE84E166}"/>
+  <tableColumns count="16">
+    <tableColumn id="1" xr3:uid="{6D5CF608-DCFD-4A92-A596-E8063172E174}" name="serial No" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{C0209DF9-846E-4857-B58B-B8541011985F}" name="runNo" dataDxfId="14"/>
+    <tableColumn id="3" xr3:uid="{0E30CBAC-72EE-4AD2-A47C-82B32671EA5E}" name="prev" dataDxfId="13"/>
+    <tableColumn id="18" xr3:uid="{2FADAE80-F4C1-47E4-9F74-0288B8A6CB62}" name="run On" dataDxfId="0"/>
+    <tableColumn id="14" xr3:uid="{0226C407-085D-4DCB-8736-D2AF531847FD}" name="final epoch" dataDxfId="12"/>
     <tableColumn id="4" xr3:uid="{336146EF-7573-4D55-988F-4943F72E43C9}" name="batch_size" dataDxfId="11"/>
     <tableColumn id="5" xr3:uid="{7D897263-E705-4F32-ADB2-D8CE05479643}" name="seq_len" dataDxfId="10"/>
     <tableColumn id="6" xr3:uid="{D1CBA8C9-7ABC-44A6-B183-A97BE80458C8}" name="h_dim" dataDxfId="9"/>
@@ -206,8 +259,9 @@
     <tableColumn id="9" xr3:uid="{85C0A2CD-07B2-40D6-A28B-AA98CF95C923}" name="learn_rate" dataDxfId="6"/>
     <tableColumn id="10" xr3:uid="{8EDFC67B-F67A-4CD4-95AF-7F2C11BDD56B}" name="lr_sched_factor" dataDxfId="5"/>
     <tableColumn id="11" xr3:uid="{EE8D34CC-48EC-4F77-BCE1-E4C06C400749}" name="lr_ched_patience" dataDxfId="4"/>
-    <tableColumn id="12" xr3:uid="{FEF81069-965A-4F7F-9A04-CDB8456ED181}" name="best train acc" dataDxfId="3"/>
-    <tableColumn id="13" xr3:uid="{C2B6B97F-D922-4447-8522-4BCAC10B9BA9}" name="best test acc" dataDxfId="2"/>
+    <tableColumn id="12" xr3:uid="{FEF81069-965A-4F7F-9A04-CDB8456ED181}" name="best test acc" dataDxfId="3"/>
+    <tableColumn id="13" xr3:uid="{C2B6B97F-D922-4447-8522-4BCAC10B9BA9}" name="best train acc" dataDxfId="2"/>
+    <tableColumn id="15" xr3:uid="{1FD8B743-0F32-4858-B944-2FAF36FA864A}" name="Notes" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -510,10 +564,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D279DA9D-5DEE-48AA-9DA5-B575201FB7DE}">
-  <dimension ref="A1:N3"/>
+  <dimension ref="A1:P13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="P13" sqref="P13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -530,11 +584,12 @@
     <col min="10" max="10" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="17" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.42578125" customWidth="1"/>
+    <col min="16" max="16" width="13.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -545,40 +600,46 @@
         <v>13</v>
       </c>
       <c r="D1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" t="s">
         <v>14</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>0</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>1</v>
       </c>
-      <c r="G1" t="s">
-        <v>2</v>
-      </c>
       <c r="H1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I1" t="s">
         <v>3</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>4</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>5</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>6</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>7</v>
-      </c>
-      <c r="M1" t="s">
-        <v>9</v>
       </c>
       <c r="N1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="O1" t="s">
+        <v>9</v>
+      </c>
+      <c r="P1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -588,41 +649,41 @@
       <c r="C2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="1">
+      <c r="F2" s="1">
         <v>256</v>
       </c>
-      <c r="F2" s="1">
+      <c r="G2" s="1">
         <v>100</v>
       </c>
-      <c r="G2" s="1">
+      <c r="H2" s="1">
         <v>512</v>
       </c>
-      <c r="H2" s="1">
-        <v>2</v>
-      </c>
       <c r="I2" s="1">
+        <v>2</v>
+      </c>
+      <c r="J2" s="1">
         <v>0.25</v>
       </c>
-      <c r="J2" s="1">
+      <c r="K2" s="1">
         <v>1E-3</v>
       </c>
-      <c r="K2" s="1">
+      <c r="L2" s="1">
         <v>0.2</v>
       </c>
-      <c r="L2" s="1">
-        <v>2</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>12</v>
+      <c r="M2" s="1">
+        <v>2</v>
       </c>
       <c r="N2" s="1">
         <v>57.2</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="O2" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -632,33 +693,492 @@
       <c r="C3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="2"/>
-      <c r="E3" s="1">
+      <c r="E3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="1">
         <v>256</v>
       </c>
-      <c r="F3" s="1">
+      <c r="G3" s="1">
         <v>64</v>
       </c>
-      <c r="G3" s="1">
+      <c r="H3" s="1">
         <v>512</v>
       </c>
-      <c r="H3" s="1">
+      <c r="I3" s="1">
         <v>3</v>
       </c>
-      <c r="I3" s="1">
-        <v>0.5</v>
-      </c>
       <c r="J3" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="K3" s="1">
         <v>1E-3</v>
       </c>
-      <c r="K3" s="1">
-        <v>0.5</v>
-      </c>
       <c r="L3" s="1">
-        <v>2</v>
-      </c>
+        <v>0.5</v>
+      </c>
+      <c r="M3" s="1">
+        <v>2</v>
+      </c>
+      <c r="N3" s="1">
+        <v>54.5</v>
+      </c>
+      <c r="O3" s="1">
+        <v>57.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="1">
+        <v>256</v>
+      </c>
+      <c r="G4" s="1">
+        <v>64</v>
+      </c>
+      <c r="H4" s="1">
+        <v>264</v>
+      </c>
+      <c r="I4" s="1">
+        <v>5</v>
+      </c>
+      <c r="J4" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="K4" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="L4" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="M4" s="1">
+        <v>2</v>
+      </c>
+      <c r="N4" s="1">
+        <v>44</v>
+      </c>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1"/>
+    </row>
+    <row r="5" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1">
+        <v>2</v>
+      </c>
+      <c r="C5" s="1">
+        <v>2</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" s="1">
+        <v>256</v>
+      </c>
+      <c r="G5" s="1">
+        <v>128</v>
+      </c>
+      <c r="H5" s="1">
+        <v>512</v>
+      </c>
+      <c r="I5" s="1">
+        <v>3</v>
+      </c>
+      <c r="J5" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="K5" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="L5" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="M5" s="1">
+        <v>2</v>
+      </c>
+      <c r="N5" s="1">
+        <v>57.1</v>
+      </c>
+      <c r="O5" s="1">
+        <v>60.8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1">
+        <v>2</v>
+      </c>
+      <c r="C6" s="1">
+        <v>3</v>
+      </c>
+      <c r="D6" s="1"/>
+      <c r="E6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" s="1">
+        <v>256</v>
+      </c>
+      <c r="G6" s="1">
+        <v>64</v>
+      </c>
+      <c r="H6" s="1">
+        <v>264</v>
+      </c>
+      <c r="I6" s="1">
+        <v>5</v>
+      </c>
+      <c r="J6" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="K6" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="L6" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="M6" s="1">
+        <v>2</v>
+      </c>
+      <c r="N6" s="1">
+        <v>47</v>
+      </c>
+      <c r="O6" s="1"/>
+      <c r="P6" s="1"/>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1">
+        <v>1</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F7" s="1">
+        <v>256</v>
+      </c>
+      <c r="G7" s="1">
+        <v>64</v>
+      </c>
+      <c r="H7" s="1">
+        <v>512</v>
+      </c>
+      <c r="I7" s="1">
+        <v>4</v>
+      </c>
+      <c r="J7" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="K7" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="L7" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="M7" s="1">
+        <v>2</v>
+      </c>
+      <c r="N7" s="1">
+        <v>55.1</v>
+      </c>
+      <c r="O7" s="1">
+        <v>60.5</v>
+      </c>
+      <c r="P7" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1">
+        <v>1</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="1"/>
+      <c r="E8" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" s="1">
+        <v>256</v>
+      </c>
+      <c r="G8" s="1">
+        <v>64</v>
+      </c>
+      <c r="H8" s="1">
+        <v>512</v>
+      </c>
+      <c r="I8" s="1">
+        <v>3</v>
+      </c>
+      <c r="J8" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="K8" s="1">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="L8" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="M8" s="1">
+        <v>2</v>
+      </c>
+      <c r="N8" s="1">
+        <v>57.2</v>
+      </c>
+      <c r="O8" s="1"/>
+      <c r="P8" s="1"/>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1">
+        <v>2</v>
+      </c>
+      <c r="C9" s="1">
+        <v>7</v>
+      </c>
+      <c r="D9" s="1"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="1">
+        <v>256</v>
+      </c>
+      <c r="G9" s="1">
+        <v>128</v>
+      </c>
+      <c r="H9" s="1">
+        <v>512</v>
+      </c>
+      <c r="I9" s="1">
+        <v>3</v>
+      </c>
+      <c r="J9" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="K9" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="L9" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="M9" s="1">
+        <v>2</v>
+      </c>
+      <c r="N9" s="1">
+        <v>58.4</v>
+      </c>
+      <c r="O9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="P9" s="1"/>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1">
+        <v>1</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="1"/>
+      <c r="E10" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F10" s="1">
+        <v>256</v>
+      </c>
+      <c r="G10" s="1">
+        <v>64</v>
+      </c>
+      <c r="H10" s="1">
+        <v>512</v>
+      </c>
+      <c r="I10" s="1">
+        <v>3</v>
+      </c>
+      <c r="J10" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="K10" s="1">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="L10" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="M10" s="1">
+        <v>2</v>
+      </c>
+      <c r="N10" s="1">
+        <v>50.4</v>
+      </c>
+      <c r="O10" s="1"/>
+      <c r="P10" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1">
+        <v>2</v>
+      </c>
+      <c r="C11" s="1">
+        <v>9</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F11" s="1">
+        <v>256</v>
+      </c>
+      <c r="G11" s="1">
+        <v>128</v>
+      </c>
+      <c r="H11" s="1">
+        <v>512</v>
+      </c>
+      <c r="I11" s="1">
+        <v>3</v>
+      </c>
+      <c r="J11" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="K11" s="1">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="L11" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="M11" s="1">
+        <v>2</v>
+      </c>
+      <c r="N11" s="1">
+        <v>49.8</v>
+      </c>
+      <c r="O11" s="1">
+        <v>57.1</v>
+      </c>
+      <c r="P11" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1">
+        <v>2</v>
+      </c>
+      <c r="C12" s="1">
+        <v>6</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E12" s="2"/>
+      <c r="F12" s="1">
+        <v>256</v>
+      </c>
+      <c r="G12" s="1">
+        <v>128</v>
+      </c>
+      <c r="H12" s="1">
+        <v>512</v>
+      </c>
+      <c r="I12" s="1">
+        <v>4</v>
+      </c>
+      <c r="J12" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="K12" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="L12" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="M12" s="1">
+        <v>2</v>
+      </c>
+      <c r="N12" s="1"/>
+      <c r="O12" s="1"/>
+      <c r="P12" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1">
+        <v>1</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E13" s="2"/>
+      <c r="F13" s="1">
+        <v>256</v>
+      </c>
+      <c r="G13" s="1">
+        <v>32</v>
+      </c>
+      <c r="H13" s="1">
+        <v>512</v>
+      </c>
+      <c r="I13" s="1">
+        <v>3</v>
+      </c>
+      <c r="J13" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="K13" s="1">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="L13" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="M13" s="1">
+        <v>2</v>
+      </c>
+      <c r="N13" s="1"/>
+      <c r="O13" s="1"/>
+      <c r="P13" s="1"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">

</xml_diff>